<commit_message>
pushing 24th aug chnages for education goal
</commit_message>
<xml_diff>
--- a/src/main/java/com/ey/test3po/testdata/TestData.xlsx
+++ b/src/main/java/com/ey/test3po/testdata/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Back Up\Project Work\Learning Stuffs\Eclipse Oxygen\3PO\src\main\java\com\ey\test3po\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satyaranjan.muduli\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9345" tabRatio="847" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9345" tabRatio="847" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="UserProfile" sheetId="25" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2664" uniqueCount="445">
   <si>
     <t>Age</t>
   </si>
@@ -1328,6 +1328,48 @@
   </si>
   <si>
     <t>62126</t>
+  </si>
+  <si>
+    <t>41083</t>
+  </si>
+  <si>
+    <t>Zero_1</t>
+  </si>
+  <si>
+    <t>44660</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>3061</t>
+  </si>
+  <si>
+    <t>Zero_2</t>
+  </si>
+  <si>
+    <t>4676</t>
+  </si>
+  <si>
+    <t>43041</t>
+  </si>
+  <si>
+    <t>Zero_3</t>
+  </si>
+  <si>
+    <t>47963</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>285</t>
+  </si>
+  <si>
+    <t>1937</t>
+  </si>
+  <si>
+    <t>3763549</t>
   </si>
 </sst>
 </file>
@@ -1438,7 +1480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1468,6 +1510,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1972,7 +2016,7 @@
       </c>
       <c r="W2" s="24"/>
       <c r="X2" s="24"/>
-      <c r="Y2" s="24" t="s">
+      <c r="Y2" s="29" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2041,7 +2085,7 @@
       <c r="V3" s="26"/>
       <c r="W3" s="24"/>
       <c r="X3" s="24"/>
-      <c r="Y3" s="24" t="s">
+      <c r="Y3" s="29" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2110,7 +2154,7 @@
       <c r="V4" s="26"/>
       <c r="W4" s="24"/>
       <c r="X4" s="24"/>
-      <c r="Y4" s="24" t="s">
+      <c r="Y4" s="29" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2183,7 +2227,7 @@
       </c>
       <c r="W5" s="26"/>
       <c r="X5" s="26"/>
-      <c r="Y5" s="24" t="s">
+      <c r="Y5" s="29" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2246,7 +2290,7 @@
       <c r="V6" s="26"/>
       <c r="W6" s="26"/>
       <c r="X6" s="26"/>
-      <c r="Y6" s="24" t="s">
+      <c r="Y6" s="29" t="s">
         <v>198</v>
       </c>
     </row>
@@ -2309,7 +2353,7 @@
       <c r="V7" s="18"/>
       <c r="W7" s="18"/>
       <c r="X7" s="18"/>
-      <c r="Y7" s="19" t="s">
+      <c r="Y7" s="30" t="s">
         <v>202</v>
       </c>
     </row>
@@ -2368,7 +2412,7 @@
       <c r="X8" s="18" t="s">
         <v>385</v>
       </c>
-      <c r="Y8" s="19" t="s">
+      <c r="Y8" s="30" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2431,7 +2475,7 @@
         <v>307</v>
       </c>
       <c r="X9" s="18"/>
-      <c r="Y9" s="19" t="s">
+      <c r="Y9" s="30" t="s">
         <v>317</v>
       </c>
     </row>
@@ -2504,7 +2548,7 @@
         <v>307</v>
       </c>
       <c r="X10" s="18"/>
-      <c r="Y10" s="19" t="s">
+      <c r="Y10" s="30" t="s">
         <v>318</v>
       </c>
     </row>
@@ -2577,7 +2621,7 @@
       </c>
       <c r="W11" s="13"/>
       <c r="X11" s="18"/>
-      <c r="Y11" s="9" t="s">
+      <c r="Y11" s="11" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2638,7 +2682,7 @@
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
       <c r="X12" s="18"/>
-      <c r="Y12" s="9" t="s">
+      <c r="Y12" s="11" t="s">
         <v>388</v>
       </c>
     </row>
@@ -2709,7 +2753,7 @@
       </c>
       <c r="W13" s="9"/>
       <c r="X13" s="18"/>
-      <c r="Y13" s="9" t="s">
+      <c r="Y13" s="11" t="s">
         <v>389</v>
       </c>
     </row>
@@ -2778,7 +2822,7 @@
       </c>
       <c r="W14" s="9"/>
       <c r="X14" s="18"/>
-      <c r="Y14" s="9" t="s">
+      <c r="Y14" s="11" t="s">
         <v>395</v>
       </c>
     </row>
@@ -2841,7 +2885,7 @@
       <c r="V15" s="9"/>
       <c r="W15" s="9"/>
       <c r="X15" s="19"/>
-      <c r="Y15" s="9" t="s">
+      <c r="Y15" s="11" t="s">
         <v>349</v>
       </c>
     </row>
@@ -2904,7 +2948,7 @@
       <c r="V16" s="9"/>
       <c r="W16" s="9"/>
       <c r="X16" s="19"/>
-      <c r="Y16" s="9" t="s">
+      <c r="Y16" s="11" t="s">
         <v>350</v>
       </c>
     </row>
@@ -2967,7 +3011,7 @@
       <c r="V17" s="9"/>
       <c r="W17" s="9"/>
       <c r="X17" s="19"/>
-      <c r="Y17" s="9" t="s">
+      <c r="Y17" s="11" t="s">
         <v>351</v>
       </c>
     </row>
@@ -3030,7 +3074,7 @@
       <c r="V18" s="9"/>
       <c r="W18" s="9"/>
       <c r="X18" s="19"/>
-      <c r="Y18" s="9" t="s">
+      <c r="Y18" s="11" t="s">
         <v>352</v>
       </c>
     </row>
@@ -3101,7 +3145,7 @@
       </c>
       <c r="W19" s="26"/>
       <c r="X19" s="26"/>
-      <c r="Y19" s="24" t="s">
+      <c r="Y19" s="29" t="s">
         <v>226</v>
       </c>
     </row>
@@ -3137,7 +3181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4659,7 +4703,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4820,7 +4864,7 @@
         <v>50</v>
       </c>
       <c r="V2" s="13"/>
-      <c r="W2" s="9" t="s">
+      <c r="W2" s="11" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4889,7 +4933,7 @@
         <v>50</v>
       </c>
       <c r="V3" s="13"/>
-      <c r="W3" s="9" t="s">
+      <c r="W3" s="11" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4958,7 +5002,7 @@
         <v>50</v>
       </c>
       <c r="V4" s="13"/>
-      <c r="W4" s="9" t="s">
+      <c r="W4" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5017,7 +5061,7 @@
       </c>
       <c r="U5" s="13"/>
       <c r="V5" s="13"/>
-      <c r="W5" s="9" t="s">
+      <c r="W5" s="11" t="s">
         <v>75</v>
       </c>
     </row>
@@ -5076,7 +5120,7 @@
       </c>
       <c r="U6" s="13"/>
       <c r="V6" s="13"/>
-      <c r="W6" s="9" t="s">
+      <c r="W6" s="11" t="s">
         <v>95</v>
       </c>
     </row>
@@ -5135,7 +5179,7 @@
       </c>
       <c r="U7" s="13"/>
       <c r="V7" s="13"/>
-      <c r="W7" s="9" t="s">
+      <c r="W7" s="11" t="s">
         <v>96</v>
       </c>
     </row>
@@ -5194,7 +5238,7 @@
       </c>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
-      <c r="W8" s="9" t="s">
+      <c r="W8" s="11" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5253,7 +5297,7 @@
       </c>
       <c r="U9" s="13"/>
       <c r="V9" s="13"/>
-      <c r="W9" s="9" t="s">
+      <c r="W9" s="11" t="s">
         <v>183</v>
       </c>
     </row>
@@ -5312,7 +5356,7 @@
       </c>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
-      <c r="W10" s="9" t="s">
+      <c r="W10" s="11" t="s">
         <v>184</v>
       </c>
     </row>
@@ -5377,7 +5421,7 @@
       </c>
       <c r="U11" s="13"/>
       <c r="V11" s="13"/>
-      <c r="W11" s="9" t="s">
+      <c r="W11" s="11" t="s">
         <v>191</v>
       </c>
     </row>
@@ -5442,7 +5486,7 @@
       </c>
       <c r="U12" s="13"/>
       <c r="V12" s="13"/>
-      <c r="W12" s="9" t="s">
+      <c r="W12" s="11" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5507,7 +5551,7 @@
       </c>
       <c r="U13" s="13"/>
       <c r="V13" s="13"/>
-      <c r="W13" s="9" t="s">
+      <c r="W13" s="11" t="s">
         <v>193</v>
       </c>
     </row>
@@ -5576,7 +5620,7 @@
         <v>50</v>
       </c>
       <c r="V14" s="13"/>
-      <c r="W14" s="9" t="s">
+      <c r="W14" s="11" t="s">
         <v>197</v>
       </c>
     </row>
@@ -5645,7 +5689,7 @@
         <v>50</v>
       </c>
       <c r="V15" s="13"/>
-      <c r="W15" s="9" t="s">
+      <c r="W15" s="11" t="s">
         <v>198</v>
       </c>
     </row>
@@ -5714,7 +5758,7 @@
         <v>50</v>
       </c>
       <c r="V16" s="13"/>
-      <c r="W16" s="9" t="s">
+      <c r="W16" s="11" t="s">
         <v>199</v>
       </c>
     </row>
@@ -5779,7 +5823,7 @@
       </c>
       <c r="U17" s="13"/>
       <c r="V17" s="13"/>
-      <c r="W17" s="9" t="s">
+      <c r="W17" s="11" t="s">
         <v>200</v>
       </c>
     </row>
@@ -5844,7 +5888,7 @@
       </c>
       <c r="U18" s="13"/>
       <c r="V18" s="13"/>
-      <c r="W18" s="9" t="s">
+      <c r="W18" s="11" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5909,7 +5953,7 @@
       </c>
       <c r="U19" s="13"/>
       <c r="V19" s="13"/>
-      <c r="W19" s="9" t="s">
+      <c r="W19" s="11" t="s">
         <v>202</v>
       </c>
     </row>
@@ -5978,7 +6022,7 @@
         <v>50</v>
       </c>
       <c r="V20" s="13"/>
-      <c r="W20" s="9" t="s">
+      <c r="W20" s="11" t="s">
         <v>206</v>
       </c>
     </row>
@@ -6047,7 +6091,7 @@
         <v>50</v>
       </c>
       <c r="V21" s="13"/>
-      <c r="W21" s="9" t="s">
+      <c r="W21" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -6116,7 +6160,7 @@
         <v>50</v>
       </c>
       <c r="V22" s="13"/>
-      <c r="W22" s="9" t="s">
+      <c r="W22" s="11" t="s">
         <v>208</v>
       </c>
     </row>
@@ -6187,7 +6231,7 @@
       <c r="V23" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="W23" s="9" t="s">
+      <c r="W23" s="11" t="s">
         <v>426</v>
       </c>
     </row>
@@ -6248,7 +6292,7 @@
       <c r="V24" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="W24" s="9" t="s">
+      <c r="W24" s="11" t="s">
         <v>310</v>
       </c>
     </row>
@@ -6319,7 +6363,7 @@
       <c r="V25" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="W25" s="9" t="s">
+      <c r="W25" s="11" t="s">
         <v>364</v>
       </c>
     </row>
@@ -6378,7 +6422,7 @@
       <c r="T26" s="13"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
-      <c r="W26" s="9" t="s">
+      <c r="W26" s="11" t="s">
         <v>361</v>
       </c>
     </row>
@@ -6447,7 +6491,7 @@
         <v>81</v>
       </c>
       <c r="V27" s="8"/>
-      <c r="W27" s="9" t="s">
+      <c r="W27" s="11" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6514,7 +6558,7 @@
         <v>67</v>
       </c>
       <c r="V28" s="13"/>
-      <c r="W28" s="9" t="s">
+      <c r="W28" s="11" t="s">
         <v>363</v>
       </c>
     </row>
@@ -6750,7 +6794,7 @@
         <v>54</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>104</v>
+        <v>444</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -6770,12 +6814,12 @@
         <v>104</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="R3" s="8"/>
       <c r="S3" s="13"/>
       <c r="T3" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="U3" s="8"/>
       <c r="V3" s="13"/>
@@ -7631,7 +7675,7 @@
         <v>50</v>
       </c>
       <c r="V2" s="13"/>
-      <c r="W2" s="9" t="s">
+      <c r="W2" s="11" t="s">
         <v>51</v>
       </c>
     </row>
@@ -7700,7 +7744,7 @@
         <v>50</v>
       </c>
       <c r="V3" s="13"/>
-      <c r="W3" s="9" t="s">
+      <c r="W3" s="11" t="s">
         <v>52</v>
       </c>
     </row>
@@ -7769,7 +7813,7 @@
         <v>50</v>
       </c>
       <c r="V4" s="13"/>
-      <c r="W4" s="9" t="s">
+      <c r="W4" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -7828,7 +7872,7 @@
       </c>
       <c r="U5" s="13"/>
       <c r="V5" s="13"/>
-      <c r="W5" s="9" t="s">
+      <c r="W5" s="11" t="s">
         <v>75</v>
       </c>
     </row>
@@ -7887,7 +7931,7 @@
       </c>
       <c r="U6" s="13"/>
       <c r="V6" s="13"/>
-      <c r="W6" s="9" t="s">
+      <c r="W6" s="11" t="s">
         <v>95</v>
       </c>
     </row>
@@ -7946,7 +7990,7 @@
       </c>
       <c r="U7" s="13"/>
       <c r="V7" s="13"/>
-      <c r="W7" s="9" t="s">
+      <c r="W7" s="11" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8005,7 +8049,7 @@
       </c>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
-      <c r="W8" s="9" t="s">
+      <c r="W8" s="11" t="s">
         <v>147</v>
       </c>
     </row>
@@ -8064,7 +8108,7 @@
       </c>
       <c r="U9" s="13"/>
       <c r="V9" s="13"/>
-      <c r="W9" s="9" t="s">
+      <c r="W9" s="11" t="s">
         <v>183</v>
       </c>
     </row>
@@ -8123,7 +8167,7 @@
       </c>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
-      <c r="W10" s="9" t="s">
+      <c r="W10" s="11" t="s">
         <v>184</v>
       </c>
     </row>
@@ -8188,7 +8232,7 @@
       </c>
       <c r="U11" s="13"/>
       <c r="V11" s="13"/>
-      <c r="W11" s="9" t="s">
+      <c r="W11" s="11" t="s">
         <v>191</v>
       </c>
     </row>
@@ -8253,7 +8297,7 @@
       </c>
       <c r="U12" s="13"/>
       <c r="V12" s="13"/>
-      <c r="W12" s="9" t="s">
+      <c r="W12" s="11" t="s">
         <v>192</v>
       </c>
     </row>
@@ -8318,7 +8362,7 @@
       </c>
       <c r="U13" s="13"/>
       <c r="V13" s="13"/>
-      <c r="W13" s="9" t="s">
+      <c r="W13" s="11" t="s">
         <v>193</v>
       </c>
     </row>
@@ -8387,7 +8431,7 @@
         <v>50</v>
       </c>
       <c r="V14" s="13"/>
-      <c r="W14" s="9" t="s">
+      <c r="W14" s="11" t="s">
         <v>197</v>
       </c>
     </row>
@@ -8456,7 +8500,7 @@
         <v>50</v>
       </c>
       <c r="V15" s="13"/>
-      <c r="W15" s="9" t="s">
+      <c r="W15" s="11" t="s">
         <v>198</v>
       </c>
     </row>
@@ -8525,7 +8569,7 @@
         <v>50</v>
       </c>
       <c r="V16" s="13"/>
-      <c r="W16" s="9" t="s">
+      <c r="W16" s="11" t="s">
         <v>199</v>
       </c>
     </row>
@@ -8590,7 +8634,7 @@
       </c>
       <c r="U17" s="13"/>
       <c r="V17" s="13"/>
-      <c r="W17" s="9" t="s">
+      <c r="W17" s="11" t="s">
         <v>200</v>
       </c>
     </row>
@@ -8655,7 +8699,7 @@
       </c>
       <c r="U18" s="13"/>
       <c r="V18" s="13"/>
-      <c r="W18" s="9" t="s">
+      <c r="W18" s="11" t="s">
         <v>201</v>
       </c>
     </row>
@@ -8720,7 +8764,7 @@
       </c>
       <c r="U19" s="13"/>
       <c r="V19" s="13"/>
-      <c r="W19" s="9" t="s">
+      <c r="W19" s="11" t="s">
         <v>202</v>
       </c>
     </row>
@@ -8789,7 +8833,7 @@
         <v>50</v>
       </c>
       <c r="V20" s="13"/>
-      <c r="W20" s="9" t="s">
+      <c r="W20" s="11" t="s">
         <v>206</v>
       </c>
     </row>
@@ -8858,7 +8902,7 @@
         <v>50</v>
       </c>
       <c r="V21" s="13"/>
-      <c r="W21" s="9" t="s">
+      <c r="W21" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -8927,7 +8971,7 @@
         <v>50</v>
       </c>
       <c r="V22" s="13"/>
-      <c r="W22" s="9" t="s">
+      <c r="W22" s="11" t="s">
         <v>208</v>
       </c>
     </row>
@@ -8998,7 +9042,7 @@
       <c r="V23" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="W23" s="9" t="s">
+      <c r="W23" s="11" t="s">
         <v>426</v>
       </c>
     </row>
@@ -9059,7 +9103,7 @@
       <c r="V24" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="W24" s="9" t="s">
+      <c r="W24" s="11" t="s">
         <v>310</v>
       </c>
     </row>
@@ -9130,7 +9174,7 @@
       <c r="V25" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="W25" s="9" t="s">
+      <c r="W25" s="11" t="s">
         <v>364</v>
       </c>
     </row>
@@ -9189,7 +9233,7 @@
       <c r="T26" s="13"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
-      <c r="W26" s="9" t="s">
+      <c r="W26" s="11" t="s">
         <v>361</v>
       </c>
     </row>
@@ -9258,7 +9302,7 @@
         <v>81</v>
       </c>
       <c r="V27" s="8"/>
-      <c r="W27" s="9" t="s">
+      <c r="W27" s="11" t="s">
         <v>362</v>
       </c>
     </row>
@@ -9325,7 +9369,7 @@
         <v>67</v>
       </c>
       <c r="V28" s="13"/>
-      <c r="W28" s="9" t="s">
+      <c r="W28" s="11" t="s">
         <v>363</v>
       </c>
     </row>
@@ -10523,7 +10567,7 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10674,11 +10718,11 @@
         <v>45</v>
       </c>
       <c r="T2" s="13"/>
-      <c r="U2" s="9" t="s">
+      <c r="U2" s="11" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
@@ -10737,11 +10781,11 @@
         <v>63</v>
       </c>
       <c r="T3" s="13"/>
-      <c r="U3" s="9" t="s">
+      <c r="U3" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>66</v>
       </c>
@@ -10800,7 +10844,7 @@
         <v>74</v>
       </c>
       <c r="T4" s="13"/>
-      <c r="U4" s="9" t="s">
+      <c r="U4" s="11" t="s">
         <v>147</v>
       </c>
     </row>
@@ -10922,13 +10966,202 @@
         <v>197</v>
       </c>
     </row>
+    <row r="7" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" s="11">
+        <v>123</v>
+      </c>
+      <c r="O7" s="11">
+        <v>123</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="S7" s="8"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="11" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="11">
+        <v>123</v>
+      </c>
+      <c r="O8" s="11">
+        <v>123</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="T8" s="13"/>
+      <c r="U8" s="11" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="11">
+        <v>123</v>
+      </c>
+      <c r="O9" s="11">
+        <v>123</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="T9" s="13"/>
+      <c r="U9" s="11" t="s">
+        <v>439</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A2:U9">
+    <sortCondition ref="U1"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1"/>
     <hyperlink ref="M3" r:id="rId2"/>
     <hyperlink ref="M4" r:id="rId3"/>
     <hyperlink ref="M5" r:id="rId4"/>
     <hyperlink ref="M6" r:id="rId5"/>
+    <hyperlink ref="M7" r:id="rId6"/>
+    <hyperlink ref="M8" r:id="rId7"/>
+    <hyperlink ref="M9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10937,7 +11170,7 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11337,13 +11570,202 @@
         <v>199</v>
       </c>
     </row>
+    <row r="7" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" s="11">
+        <v>123</v>
+      </c>
+      <c r="O7" s="11">
+        <v>123</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" s="8"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="11" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="11">
+        <v>123</v>
+      </c>
+      <c r="O8" s="11">
+        <v>123</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="T8" s="13"/>
+      <c r="U8" s="11" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="11">
+        <v>123</v>
+      </c>
+      <c r="O9" s="11">
+        <v>123</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="T9" s="13"/>
+      <c r="U9" s="11" t="s">
+        <v>439</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A2:U9">
+    <sortCondition ref="U1"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1"/>
     <hyperlink ref="M3" r:id="rId2"/>
     <hyperlink ref="M4" r:id="rId3"/>
     <hyperlink ref="M5" r:id="rId4"/>
     <hyperlink ref="M6" r:id="rId5"/>
+    <hyperlink ref="M7" r:id="rId6"/>
+    <hyperlink ref="M8" r:id="rId7"/>
+    <hyperlink ref="M9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>